<commit_message>
add new data from 2023
</commit_message>
<xml_diff>
--- a/votesheets/gaza votes 2023.xlsx
+++ b/votesheets/gaza votes 2023.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/150a535b2faa7c4c/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/athan/Projects/GazaLegislativeScorecard/votesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{809505E2-A719-495B-91EB-EB8089631BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD50E5A-18AE-8547-90E0-F32B7ACDF552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DFE9EA50-9290-4683-BAAE-A81A761F95FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26680" windowHeight="15740" xr2:uid="{DFE9EA50-9290-4683-BAAE-A81A761F95FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t>HR2670 is NDAA2023. Included in its provisions is an increase of ~$150M immediately in aid to Israel, an extension of all existing aid, and and an affirmative promise to meet Israel's arms needs following a DoD assessment.</t>
   </si>
@@ -92,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">SRES417 condemns Hamas for October 7 and expresses the sense of the Senate that Israel has a right to defend itself, as well as the sense of the senate that Israel should be provided with expedited access to military transfers </t>
-  </si>
-  <si>
-    <t>.1.5</t>
   </si>
   <si>
     <t>SRES413 condems specifically foreign nationals in the United States who have  endorsed Hamas</t>
@@ -914,349 +910,349 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21DB431-E2B8-4719-BEAB-AF64A6DDA01B}">
   <dimension ref="A1:DE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="O11" zoomScale="165" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="32.3984375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:109" ht="90" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AA1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AB1" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC1" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AE1" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AG1" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AI1" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AJ1" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AK1" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AL1" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AM1" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AN1" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AO1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AP1" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AQ1" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AS1" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AT1" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AU1" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AV1" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AW1" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AX1" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AY1" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AZ1" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="BA1" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="BB1" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="BC1" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BD1" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BE1" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BF1" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BG1" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BH1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BI1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BJ1" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BK1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BL1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BM1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BN1" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BO1" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BP1" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BQ1" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BR1" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BS1" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BT1" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BU1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BV1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BW1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BX1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BY1" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BZ1" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="CA1" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="CB1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="CC1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="CD1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="CE1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="CF1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CG1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="CH1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="CI1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="CJ1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="CK1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="CL1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="CM1" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="CN1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="CO1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="CP1" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="CQ1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="CR1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="CS1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="CT1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="CU1" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="CV1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="CW1" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="CX1" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="CY1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="CZ1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="DA1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="DB1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="DC1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="DD1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:109" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:109" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>45215</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -1577,12 +1573,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>45216</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -1903,12 +1899,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>45216</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -2229,12 +2225,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>45216</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -2555,12 +2551,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>45216</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -2881,9 +2877,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:109" ht="78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:109" ht="90" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -3204,9 +3200,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:109" ht="39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:109" ht="45" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3">
         <v>-0.4</v>
@@ -3527,9 +3523,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:109" ht="52" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:109" ht="60" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -3850,12 +3846,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:109" ht="39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:109" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>45216</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -4176,12 +4172,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:109" ht="26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:109" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>45216</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -4502,12 +4498,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:109" ht="52" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:109" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>45217</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -4828,9 +4824,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:109" ht="39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:109" ht="45" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -5151,9 +5147,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:109" ht="39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:109" ht="45" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -5221,8 +5217,8 @@
       <c r="X14" s="2">
         <v>1.5</v>
       </c>
-      <c r="Y14" s="2" t="s">
-        <v>11</v>
+      <c r="Y14" s="2">
+        <v>1.5</v>
       </c>
       <c r="Z14" s="2">
         <v>0</v>
@@ -5474,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:109" ht="91" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:109" ht="105" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
@@ -5797,7 +5793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:109" ht="65" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:109" ht="75" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
@@ -6121,7 +6117,7 @@
       </c>
       <c r="DE16" s="2"/>
     </row>
-    <row r="17" spans="2:108" ht="39" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:108" ht="45" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
@@ -6444,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:108" ht="26" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:108" ht="30" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
@@ -6767,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:108" ht="39" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:108" ht="60" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
@@ -7090,7 +7086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:108" ht="39" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:108" ht="45" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
@@ -7413,7 +7409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:108" ht="39" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:108" ht="45" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
@@ -7736,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:108" ht="52" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:108" ht="60" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
@@ -8059,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:108" ht="78" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:108" ht="90" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>2</v>
       </c>
@@ -8382,7 +8378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:108" ht="65" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:108" ht="75" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>1</v>
       </c>
@@ -8705,7 +8701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:108" ht="91" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:108" ht="105" x14ac:dyDescent="0.2">
       <c r="B25" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>